<commit_message>
Modification mineure de Taskliste3.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Taskliste3.xlsx
+++ b/Documentation/Taskliste3.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanhollet/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDant\ProjectWatch\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -48,17 +48,10 @@
 choix de type de cadrans</t>
   </si>
   <si>
-    <t>Code écrit afin de créer le programme de la montre analog</t>
-  </si>
-  <si>
     <t>Modification des programmes afin d'éviter les conflits de threads dans les programmes</t>
   </si>
   <si>
     <t>Code écrit afin d'afficher plusieurs cadrans analogiques dans la même fenêtre</t>
-  </si>
-  <si>
-    <t>Recherche de documentation sur Internet afin d'implémenter la montre analogue
-dans une fenêtre séparée</t>
   </si>
   <si>
     <t>Recherche de documentation sur Internet afin d'implémenter la montre analogue
@@ -82,12 +75,19 @@
   </si>
   <si>
     <t>Mise à jour des différents fichiers de documentation</t>
+  </si>
+  <si>
+    <t>Recherche de la documentation sur Internet afin d'implémenter la montre analogue
+dans une fenêtre séparée</t>
+  </si>
+  <si>
+    <t>Code écrit afin de créer le programme de la montre analogue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -141,6 +141,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -408,21 +411,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="71.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="71.796875" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,64 +442,64 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+    <row r="9" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>